<commit_message>
#update fix file can't open and group
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -30,553 +30,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Thai Phuong</author>
-    <author>Jenny Ngan</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Partner Code</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Partner Code Của Ac Ref</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Partner EN Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Inv</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Invoice No</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Số billing no - SOA - CR</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Billing date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Due Date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Alex:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
- Unpaid Amount của Hóa Đơn (VAT Invoice Type là Invoice) Trên Phiếu Billing</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Jenny Ngan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
- Sum (Unpaid Amount )của OBH (VAT Invoice Type là InvoiceTempt) trên 1 chứng từ billing SOA/DN</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-= Remain debit + remain OBH</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-- Đối với chưng từ billing là DN thì sẽ hiện số job tương ứng
-- SOA thì Để trống </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Thai Phuong:
-- Đối với chưng từ billing là DN thì sẽ hiện số MBL tương ứng
-- SOA thì Để trống</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Thai Phuong:
-- Đối với chưng từ billing là DN thì sẽ hiện số HBL tương ứng
-- SOA thì Để trống</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Thai Phuong:
-- Đối với chưng từ billing là DN thì sẽ hiện số Custom No
-- SOA thì Để trống</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Sale Man của khách hàng</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Creator của Billing No</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Paid Amount  của Hóa đơn</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Paid Amount của payment OBH</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Jenny Ngan:
-Paid Date (payment Date)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Jenny Ngan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-Receipt NO
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Remain của payment debit</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Remain của Payment OBH</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="R6" authorId="0" shapeId="0">
       <text>
         <r>
@@ -808,7 +263,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,17 +341,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1135,6 +579,56 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1195,56 +689,6 @@
     <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1667,131 +1111,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35" t="s">
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="30" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="38" t="s">
+      <c r="W3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="X3" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1810,17 +1254,17 @@
       <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="37" t="s">
+      <c r="R4" s="49"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="37" t="s">
+      <c r="U4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
     </row>
     <row r="5" spans="1:24" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1895,105 +1339,105 @@
     </row>
     <row r="6" spans="1:24" s="7" customFormat="1" ht="39">
       <c r="A6" s="15"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="44" t="s">
+      <c r="M6" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="46" t="s">
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="46" t="s">
+      <c r="Q6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="R6" s="46" t="s">
+      <c r="R6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="43" t="s">
+      <c r="S6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="43" t="s">
+      <c r="T6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="U6" s="43" t="s">
+      <c r="U6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="43" t="s">
+      <c r="V6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="43" t="s">
+      <c r="W6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="X6" s="43" t="s">
+      <c r="X6" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="7" customFormat="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="51" t="s">
+      <c r="M7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="52" t="s">
+      <c r="N7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="52" t="s">
+      <c r="O7" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
     </row>
     <row r="8" spans="1:24" s="14" customFormat="1">
       <c r="B8" s="8"/>
@@ -2039,11 +1483,6 @@
   </sheetData>
   <autoFilter ref="B5:X6"/>
   <mergeCells count="21">
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -2060,6 +1499,11 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:R4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>

</xml_diff>

<commit_message>
#update update group data and format excel
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -40,7 +40,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Thai Phuong:</t>
         </r>
@@ -49,7 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -334,13 +334,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -617,6 +617,66 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -628,66 +688,6 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1111,131 +1111,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="53" t="s">
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="49"/>
+      <c r="R3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="30" t="s">
+      <c r="U3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="32" t="s">
+      <c r="W3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="32" t="s">
+      <c r="X3" s="52" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
       <c r="L4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1254,17 +1254,17 @@
       <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="31" t="s">
+      <c r="R4" s="45"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="31" t="s">
+      <c r="U4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
     </row>
     <row r="5" spans="1:24" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1483,6 +1483,11 @@
   </sheetData>
   <autoFilter ref="B5:X6"/>
   <mergeCells count="21">
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -1499,11 +1504,6 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>

</xml_diff>

<commit_message>
#commit feature/hotfix/Update-Data-Payment-List-And-Export update filter data and data export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -26,40 +26,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Thai Phuong</author>
-  </authors>
-  <commentList>
-    <comment ref="R6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
@@ -263,7 +229,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,19 +294,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -579,44 +532,56 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -676,18 +641,6 @@
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1072,11 +1025,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
@@ -1110,132 +1063,132 @@
     <col min="25" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:48">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
     </row>
-    <row r="2" spans="1:24">
-      <c r="B2" s="33" t="s">
+    <row r="2" spans="1:48">
+      <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:48" ht="15" customHeight="1">
+      <c r="B3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49" t="s">
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="44" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="50" t="s">
+      <c r="T3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="50" t="s">
+      <c r="U3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="52" t="s">
+      <c r="V3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="52" t="s">
+      <c r="X3" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
+    <row r="4" spans="1:48">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1254,19 +1207,19 @@
       <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="45"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="51" t="s">
+      <c r="R4" s="49"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="51" t="s">
+      <c r="U4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="53"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1">
+    <row r="5" spans="1:48" s="6" customFormat="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1337,7 +1290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="7" customFormat="1" ht="39">
+    <row r="6" spans="1:48" s="7" customFormat="1" ht="39">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
         <v>29</v>
@@ -1404,8 +1357,32 @@
       <c r="X6" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="15"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
     </row>
-    <row r="7" spans="1:24" s="7" customFormat="1">
+    <row r="7" spans="1:48" s="7" customFormat="1">
       <c r="A7" s="15"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -1438,8 +1415,32 @@
       <c r="V7" s="26"/>
       <c r="W7" s="26"/>
       <c r="X7" s="26"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="15"/>
+      <c r="AN7" s="15"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="15"/>
+      <c r="AQ7" s="15"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
     </row>
-    <row r="8" spans="1:24" s="14" customFormat="1">
+    <row r="8" spans="1:48" s="14" customFormat="1">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
@@ -1483,11 +1484,6 @@
   </sheetData>
   <autoFilter ref="B5:X6"/>
   <mergeCells count="21">
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -1504,6 +1500,11 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:R4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>
@@ -1529,6 +1530,5 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#update fix search data and add field excel export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -214,6 +214,30 @@
   </si>
   <si>
     <t>{SumTotalAmount}</t>
+  </si>
+  <si>
+    <t>{SoaNodt}</t>
+  </si>
+  <si>
+    <t>{JobNodt}</t>
+  </si>
+  <si>
+    <t>{MBLdt}</t>
+  </si>
+  <si>
+    <t>{HBLdt}</t>
+  </si>
+  <si>
+    <t>{CustomNodt}</t>
+  </si>
+  <si>
+    <t>{BillingDatedt}</t>
+  </si>
+  <si>
+    <t>{InvoiceDatedt}</t>
+  </si>
+  <si>
+    <t>{InvoiceNodt}</t>
   </si>
 </sst>
 </file>
@@ -324,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +388,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,44 +550,66 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,65 +622,43 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1064,131 +1082,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:48">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
     </row>
     <row r="3" spans="1:48" ht="15" customHeight="1">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="53" t="s">
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="35"/>
+      <c r="R3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="30" t="s">
+      <c r="U3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="32" t="s">
+      <c r="W3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="32" t="s">
+      <c r="X3" s="38" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:48">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1207,17 +1225,17 @@
       <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="31" t="s">
+      <c r="R4" s="31"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="31" t="s">
+      <c r="U4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
     </row>
     <row r="5" spans="1:48" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1292,69 +1310,69 @@
     </row>
     <row r="6" spans="1:48" s="7" customFormat="1" ht="39">
       <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22" t="s">
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="22" t="s">
+      <c r="Q6" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="19" t="s">
+      <c r="S6" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="T6" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="U6" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="19" t="s">
+      <c r="V6" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="19" t="s">
+      <c r="W6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="X6" s="19" t="s">
+      <c r="X6" s="50" t="s">
         <v>48</v>
       </c>
       <c r="Y6" s="15"/>
@@ -1384,37 +1402,53 @@
     </row>
     <row r="7" spans="1:48" s="7" customFormat="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="44"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="28" t="s">
+      <c r="N7" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="28" t="s">
+      <c r="O7" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="T7" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
       <c r="AA7" s="15"/>
@@ -1484,6 +1518,11 @@
   </sheetData>
   <autoFilter ref="B5:X6"/>
   <mergeCells count="21">
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -1500,11 +1539,6 @@
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>

</xml_diff>

<commit_message>
#update tinh cong no tien usd
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -15,7 +15,7 @@
     <sheet name="FWD" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FWD!$B$5:$X$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FWD!$B$5:$AA$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Công nợ còn lại</t>
   </si>
   <si>
-    <t>Tổng số tiền</t>
-  </si>
-  <si>
     <t>Số Ref. / Số Job.</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>{RemainDb}</t>
   </si>
   <si>
-    <t>{ReamainOBH}</t>
-  </si>
-  <si>
     <t>{TotalAmount}</t>
   </si>
   <si>
@@ -238,6 +232,39 @@
   </si>
   <si>
     <t>{InvoiceNodt}</t>
+  </si>
+  <si>
+    <t>Dịch vụ [usd]</t>
+  </si>
+  <si>
+    <t>Chi hộ [usd]</t>
+  </si>
+  <si>
+    <t>Tổng số tiền [vnd]</t>
+  </si>
+  <si>
+    <t>Tổng số tiền [usd]</t>
+  </si>
+  <si>
+    <t>{TotalAmountUsd}</t>
+  </si>
+  <si>
+    <t>{SumTotalAmountUsd}</t>
+  </si>
+  <si>
+    <t>{RemainDbUsd}</t>
+  </si>
+  <si>
+    <t>{SumRemainDbUsd}</t>
+  </si>
+  <si>
+    <t>{SumRemainOBHUsd}</t>
+  </si>
+  <si>
+    <t>{RemainOBHUsd}</t>
+  </si>
+  <si>
+    <t>{RemainOBH}</t>
   </si>
 </sst>
 </file>
@@ -515,7 +542,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,78 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -660,6 +615,85 @@
     <xf numFmtId="166" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1047,7 +1081,7 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AV8"/>
+  <dimension ref="A1:AY8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
@@ -1074,170 +1108,190 @@
     <col min="15" max="15" width="14" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="16.36328125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.1796875" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.81640625" style="1"/>
+    <col min="18" max="19" width="11.1796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
+    <col min="22" max="24" width="16.36328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.1796875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:51">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
     </row>
-    <row r="2" spans="1:48">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:51">
+      <c r="B2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
     </row>
-    <row r="3" spans="1:48" ht="15" customHeight="1">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="1:51" ht="15" customHeight="1">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35" t="s">
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="30" t="s">
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="W3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="X3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="Y3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="Z3" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="38" t="s">
+      <c r="AA3" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="38" t="s">
+    </row>
+    <row r="4" spans="1:51">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="50"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
     </row>
-    <row r="4" spans="1:48">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-    </row>
-    <row r="5" spans="1:48" s="6" customFormat="1">
+    <row r="5" spans="1:51" s="6" customFormat="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1286,98 +1340,107 @@
       <c r="Q5" s="5">
         <v>16</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
         <v>17</v>
       </c>
-      <c r="S5" s="5">
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
         <v>18</v>
       </c>
-      <c r="T5" s="5">
+      <c r="W5" s="5">
         <v>19</v>
       </c>
-      <c r="U5" s="5">
+      <c r="X5" s="5">
         <v>20</v>
       </c>
-      <c r="V5" s="5">
+      <c r="Y5" s="5">
         <v>21</v>
       </c>
-      <c r="W5" s="5">
+      <c r="Z5" s="5">
         <v>22</v>
       </c>
-      <c r="X5" s="5">
+      <c r="AA5" s="5">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:48" s="7" customFormat="1" ht="39">
+    <row r="6" spans="1:51" s="7" customFormat="1" ht="39">
       <c r="A6" s="15"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="E6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="F6" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="G6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="H6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="I6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="J6" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="K6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="L6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="51" t="s">
+      <c r="M6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="53" t="s">
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="R6" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6" s="50" t="s">
+      <c r="U6" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="50" t="s">
+      <c r="X6" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="U6" s="50" t="s">
+      <c r="Y6" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="50" t="s">
+      <c r="Z6" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="50" t="s">
+      <c r="AA6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="X6" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
       <c r="AB6" s="15"/>
       <c r="AC6" s="15"/>
       <c r="AD6" s="15"/>
@@ -1399,59 +1462,62 @@
       <c r="AT6" s="15"/>
       <c r="AU6" s="15"/>
       <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
+      <c r="AY6" s="15"/>
     </row>
-    <row r="7" spans="1:48" s="7" customFormat="1">
+    <row r="7" spans="1:51" s="7" customFormat="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="45" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="W7" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="45" t="s">
+      <c r="X7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="T7" s="45" t="s">
+      <c r="Y7" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="U7" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="V7" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
       <c r="AB7" s="15"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
@@ -1473,12 +1539,15 @@
       <c r="AT7" s="15"/>
       <c r="AU7" s="15"/>
       <c r="AV7" s="15"/>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15"/>
+      <c r="AY7" s="15"/>
     </row>
-    <row r="8" spans="1:48" s="14" customFormat="1">
+    <row r="8" spans="1:51" s="14" customFormat="1">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
@@ -1486,46 +1555,58 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="M8" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="T8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
+      <c r="U8" s="56" t="s">
+        <v>72</v>
+      </c>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:X6"/>
-  <mergeCells count="21">
+  <autoFilter ref="B5:AA6"/>
+  <mergeCells count="22">
+    <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="T3:T4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="P3:S3"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="B1:Z1"/>
+    <mergeCell ref="B2:Z2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -1537,20 +1618,18 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:R4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3">
+  <conditionalFormatting sqref="V3">
     <cfRule type="duplicateValues" dxfId="8" priority="9" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G3 F4 F6:G6 F8:G8">
     <cfRule type="duplicateValues" dxfId="7" priority="15" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="6" priority="16" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3 S6:U6 S8:U8">
+  <conditionalFormatting sqref="V3 V6:X6 V8:X8">
     <cfRule type="duplicateValues" dxfId="5" priority="23" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="4" priority="24" stopIfTrue="1"/>
   </conditionalFormatting>
@@ -1558,7 +1637,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="2" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:U7">
+  <conditionalFormatting sqref="V7:X7">
     <cfRule type="duplicateValues" dxfId="1" priority="3" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#update sap xep lai thu tu cot trong file
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -615,68 +615,78 @@
     <xf numFmtId="166" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -684,16 +694,6 @@
     <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1108,8 +1108,8 @@
     <col min="15" max="15" width="14" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.1796875" style="1" customWidth="1"/>
     <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
     <col min="22" max="24" width="16.36328125" style="1" customWidth="1"/>
     <col min="25" max="25" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
@@ -1118,119 +1118,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="1:51">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
     </row>
     <row r="3" spans="1:51" ht="15" customHeight="1">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="J3" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="K3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="30" t="s">
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="49" t="s">
+      <c r="Q3" s="33"/>
+      <c r="R3" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="S3" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="52"/>
+      <c r="U3" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="51" t="s">
+      <c r="W3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="51" t="s">
+      <c r="X3" s="55" t="s">
         <v>16</v>
       </c>
       <c r="Y3" s="53" t="s">
@@ -1244,16 +1246,16 @@
       </c>
     </row>
     <row r="4" spans="1:51">
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1272,19 +1274,19 @@
       <c r="Q4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="51"/>
+      <c r="S4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="52" t="s">
+      <c r="U4" s="35"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="X4" s="52" t="s">
+      <c r="X4" s="56" t="s">
         <v>26</v>
       </c>
       <c r="Y4" s="54"/>
@@ -1340,11 +1342,11 @@
       <c r="Q5" s="5">
         <v>16</v>
       </c>
-      <c r="R5" s="5"/>
+      <c r="R5" s="5">
+        <v>17</v>
+      </c>
       <c r="S5" s="5"/>
-      <c r="T5" s="5">
-        <v>17</v>
-      </c>
+      <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5">
         <v>18</v>
@@ -1411,16 +1413,16 @@
       <c r="Q6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="R6" s="55" t="s">
+      <c r="R6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="S6" s="55" t="s">
+      <c r="T6" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="T6" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="U6" s="55" t="s">
+      <c r="U6" s="30" t="s">
         <v>71</v>
       </c>
       <c r="V6" s="26" t="s">
@@ -1574,16 +1576,16 @@
       <c r="Q8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="R8" s="56" t="s">
+      <c r="R8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="56" t="s">
+      <c r="T8" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="U8" s="56" t="s">
+      <c r="U8" s="31" t="s">
         <v>72</v>
       </c>
       <c r="V8" s="11"/>
@@ -1595,14 +1597,15 @@
     </row>
   </sheetData>
   <autoFilter ref="B5:AA6"/>
-  <mergeCells count="22">
+  <mergeCells count="23">
     <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="B1:Z1"/>

</xml_diff>

<commit_message>
#update sum advance column
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>{PartnerNameAdv}</t>
+  </si>
+  <si>
+    <t>{SumAdvanceAmount}</t>
   </si>
 </sst>
 </file>
@@ -747,18 +750,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="39" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -800,33 +830,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1257,168 +1260,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
     </row>
     <row r="2" spans="1:56">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="65" t="s">
+      <c r="I3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="47" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="65" t="s">
+      <c r="P3" s="53"/>
+      <c r="Q3" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="67"/>
-      <c r="U3" s="49" t="s">
+      <c r="T3" s="54"/>
+      <c r="U3" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="V3" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="W3" s="49" t="s">
+      <c r="W3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="49" t="s">
+      <c r="X3" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="Y3" s="51" t="s">
+      <c r="Y3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="70" t="s">
+      <c r="Z3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="70" t="s">
+      <c r="AA3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="68" t="s">
+      <c r="AB3" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="72" t="s">
+      <c r="AC3" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="AD3" s="72" t="s">
+      <c r="AD3" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="AE3" s="68" t="s">
+      <c r="AE3" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="68" t="s">
+      <c r="AF3" s="47" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:56">
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1437,30 +1440,30 @@
       <c r="P4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="56"/>
       <c r="S4" s="45" t="s">
         <v>67</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="71" t="s">
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="71" t="s">
+      <c r="AA4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="58"/>
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
     </row>
     <row r="5" spans="1:56" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1844,7 +1847,9 @@
       <c r="Q9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="12"/>
+      <c r="R9" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="S9" s="31" t="s">
         <v>74</v>
       </c>
@@ -1869,18 +1874,6 @@
   </sheetData>
   <autoFilter ref="B5:AF6"/>
   <mergeCells count="28">
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="Y3:Y4"/>
@@ -1897,6 +1890,18 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="R3:R4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G3 F4">
     <cfRule type="duplicateValues" dxfId="9" priority="10" stopIfTrue="1"/>

</xml_diff>

<commit_message>
#update fix account no and revert advance data
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Customer in payment history" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>{SumAdvanceAmountUsd}</t>
+  </si>
+  <si>
+    <t>{TotalAmountAdv}</t>
+  </si>
+  <si>
+    <t>{TotalAmountUsdAdv}</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,87 +715,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -833,6 +758,91 @@
     <xf numFmtId="37" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="37" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1128,199 +1138,199 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="1" customWidth="1"/>
-    <col min="18" max="19" width="11.1796875" style="1" customWidth="1"/>
-    <col min="20" max="21" width="14.453125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1796875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.90625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.453125" style="1" customWidth="1"/>
-    <col min="25" max="27" width="16.36328125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.1796875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1796875" style="1" customWidth="1"/>
-    <col min="31" max="32" width="12.1796875" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.81640625" style="1"/>
+    <col min="14" max="14" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="1" customWidth="1"/>
+    <col min="18" max="19" width="11.140625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="14.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="16.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
+    <col min="31" max="32" width="12.140625" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:56">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="42" t="s">
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="32" t="s">
+      <c r="O3" s="56"/>
+      <c r="P3" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="38" t="s">
+      <c r="S3" s="57"/>
+      <c r="T3" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="38" t="s">
+      <c r="U3" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="W3" s="38" t="s">
+      <c r="W3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="X3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="Y3" s="43" t="s">
+      <c r="Y3" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="Z3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="34" t="s">
+      <c r="AA3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="30" t="s">
+      <c r="AB3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="40" t="s">
+      <c r="AC3" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="AD3" s="40" t="s">
+      <c r="AD3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AE3" s="30" t="s">
+      <c r="AE3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="30" t="s">
+      <c r="AF3" s="50" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:56">
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1339,31 +1349,31 @@
       <c r="O4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="39"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="59"/>
       <c r="R4" s="29" t="s">
         <v>64</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="35" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="AA4" s="35" t="s">
+      <c r="AA4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
+      <c r="AB4" s="51"/>
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
     </row>
     <row r="5" spans="1:56" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1462,16 +1472,16 @@
     </row>
     <row r="6" spans="1:56" s="7" customFormat="1">
       <c r="A6" s="15"/>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="22" t="s">
@@ -1480,59 +1490,59 @@
       <c r="G6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="60" t="s">
+      <c r="K6" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="62" t="s">
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="O6" s="62" t="s">
+      <c r="O6" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="P6" s="63" t="s">
+      <c r="P6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="64" t="s">
+      <c r="Q6" s="36"/>
+      <c r="R6" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="S6" s="64" t="s">
+      <c r="S6" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="T6" s="65" t="s">
+      <c r="T6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="65"/>
-      <c r="V6" s="66" t="s">
+      <c r="U6" s="38"/>
+      <c r="V6" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="W6" s="59" t="s">
+      <c r="W6" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="67" t="s">
+      <c r="X6" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="Y6" s="57" t="s">
+      <c r="Y6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="Z6" s="57" t="s">
+      <c r="Z6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AA6" s="57" t="s">
+      <c r="AA6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AB6" s="57" t="s">
+      <c r="AB6" s="30" t="s">
         <v>43</v>
       </c>
       <c r="AC6" s="22" t="s">
@@ -1592,12 +1602,12 @@
       <c r="G7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68" t="s">
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="68" t="s">
+      <c r="K7" s="41" t="s">
         <v>47</v>
       </c>
       <c r="L7" s="20" t="s">
@@ -1606,17 +1616,17 @@
       <c r="M7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="X7" s="69"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
       <c r="Y7" s="16" t="s">
         <v>58</v>
       </c>
@@ -1674,27 +1684,31 @@
       <c r="G8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="71"/>
-      <c r="Q8" s="73" t="s">
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="71"/>
-      <c r="U8" s="72" t="s">
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="U8" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="V8" s="71"/>
-      <c r="W8" s="71"/>
-      <c r="X8" s="71"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
       <c r="Y8" s="26"/>
       <c r="Z8" s="26"/>
       <c r="AA8" s="26"/>
@@ -1762,7 +1776,7 @@
       <c r="P9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="Q9" s="74" t="s">
+      <c r="Q9" s="47" t="s">
         <v>95</v>
       </c>
       <c r="R9" s="21" t="s">
@@ -1774,7 +1788,7 @@
       <c r="T9" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="U9" s="75" t="s">
+      <c r="U9" s="48" t="s">
         <v>96</v>
       </c>
       <c r="V9" s="21"/>

</xml_diff>

<commit_message>
#update total amount row missed
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210"/>
   </bookViews>
   <sheets>
     <sheet name="Customer in payment history" sheetId="1" r:id="rId1"/>
@@ -759,18 +759,45 @@
     <xf numFmtId="37" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -815,33 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1138,198 +1138,198 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="13.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.7265625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15.453125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.26953125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="16" width="16.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="1" customWidth="1"/>
-    <col min="18" max="19" width="14.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" style="1" customWidth="1"/>
-    <col min="25" max="27" width="16.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="12.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="12.85546875" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="1"/>
+    <col min="14" max="16" width="16.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.26953125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="14.7265625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1796875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="16.453125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.1796875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1796875" style="1" customWidth="1"/>
+    <col min="32" max="32" width="12.81640625" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:56">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="57"/>
-      <c r="AE2" s="57"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="50" t="s">
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="69" t="s">
+      <c r="O3" s="56"/>
+      <c r="P3" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="71"/>
-      <c r="T3" s="52" t="s">
+      <c r="S3" s="57"/>
+      <c r="T3" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="52" t="s">
+      <c r="V3" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="52" t="s">
+      <c r="X3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="Y3" s="54" t="s">
+      <c r="Y3" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="74" t="s">
+      <c r="Z3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="74" t="s">
+      <c r="AA3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="72" t="s">
+      <c r="AB3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="76" t="s">
+      <c r="AC3" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="AD3" s="76" t="s">
+      <c r="AD3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AE3" s="72" t="s">
+      <c r="AE3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="72" t="s">
+      <c r="AF3" s="50" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:56">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1348,31 +1348,31 @@
       <c r="O4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="59"/>
       <c r="R4" s="29" t="s">
         <v>64</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="75" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="AA4" s="75" t="s">
+      <c r="AA4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
+      <c r="AB4" s="51"/>
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
     </row>
     <row r="5" spans="1:56" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1805,18 +1805,6 @@
   </sheetData>
   <autoFilter ref="B5:AF6"/>
   <mergeCells count="28">
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="Y3:Y4"/>
@@ -1833,6 +1821,18 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="U3:U4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#update #16565 and export soa customer
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -32,9 +32,6 @@
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
   <si>
-    <t>Từ ngày ____ đến ngày ______</t>
-  </si>
-  <si>
     <t>Mã số thuế
 [đối tượng cha]</t>
   </si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>{TotalAmountUsdAdv}</t>
+  </si>
+  <si>
+    <t>{RangeDate}</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1132,7 @@
   <dimension ref="A1:BD9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="2" spans="1:56">
       <c r="B2" s="66" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -1238,87 +1238,87 @@
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1">
       <c r="B3" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="D3" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="F3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="G3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="76" t="s">
-        <v>7</v>
-      </c>
       <c r="H3" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="J3" s="62" t="s">
         <v>10</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>11</v>
       </c>
       <c r="K3" s="56"/>
       <c r="L3" s="56"/>
       <c r="M3" s="57"/>
       <c r="N3" s="62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O3" s="56"/>
       <c r="P3" s="52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q3" s="58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R3" s="56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S3" s="57"/>
       <c r="T3" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U3" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V3" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="W3" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="X3" s="58" t="s">
-        <v>76</v>
-      </c>
       <c r="Y3" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="54" t="s">
+      <c r="AA3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="54" t="s">
+      <c r="AB3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="50" t="s">
+      <c r="AC3" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD3" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD3" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AF3" s="50" t="s">
         <v>17</v>
-      </c>
-      <c r="AF3" s="50" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:56">
@@ -1331,30 +1331,30 @@
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="P4" s="53"/>
       <c r="Q4" s="59"/>
       <c r="R4" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="T4" s="59"/>
       <c r="U4" s="59"/>
@@ -1363,10 +1363,10 @@
       <c r="X4" s="59"/>
       <c r="Y4" s="64"/>
       <c r="Z4" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA4" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB4" s="51"/>
       <c r="AC4" s="61"/>
@@ -1472,89 +1472,89 @@
     <row r="6" spans="1:56" s="7" customFormat="1">
       <c r="A6" s="15"/>
       <c r="B6" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="G6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="J6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="K6" s="33" t="s">
         <v>36</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>37</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
       <c r="N6" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="36" t="s">
         <v>48</v>
-      </c>
-      <c r="O6" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="P6" s="36" t="s">
-        <v>49</v>
       </c>
       <c r="Q6" s="36"/>
       <c r="R6" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S6" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T6" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U6" s="38"/>
       <c r="V6" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="W6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="W6" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="X6" s="40" t="s">
-        <v>78</v>
-      </c>
       <c r="Y6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="Z6" s="30" t="s">
+      <c r="AA6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AA6" s="30" t="s">
+      <c r="AB6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AB6" s="30" t="s">
+      <c r="AC6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE6" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AC6" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD6" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE6" s="22" t="s">
+      <c r="AF6" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="AF6" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="AG6" s="15"/>
       <c r="AH6" s="15"/>
@@ -1584,36 +1584,36 @@
     <row r="7" spans="1:56" s="7" customFormat="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>63</v>
-      </c>
       <c r="G7" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
       <c r="J7" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="41" t="s">
-        <v>47</v>
-      </c>
       <c r="L7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="42"/>
@@ -1627,16 +1627,16 @@
       <c r="W7" s="42"/>
       <c r="X7" s="42"/>
       <c r="Y7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="Z7" s="16" t="s">
+      <c r="AA7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AA7" s="16" t="s">
+      <c r="AB7" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="AB7" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="AC7" s="19"/>
       <c r="AD7" s="19"/>
@@ -1670,18 +1670,18 @@
     <row r="8" spans="1:56" s="7" customFormat="1">
       <c r="A8" s="15"/>
       <c r="B8" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
       <c r="G8" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
@@ -1692,18 +1692,18 @@
       <c r="N8" s="44"/>
       <c r="O8" s="44"/>
       <c r="P8" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q8" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R8" s="44"/>
       <c r="S8" s="44"/>
       <c r="T8" s="49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U8" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V8" s="44"/>
       <c r="W8" s="44"/>
@@ -1714,7 +1714,7 @@
       <c r="AB8" s="26"/>
       <c r="AC8" s="26"/>
       <c r="AD8" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AE8" s="26"/>
       <c r="AF8" s="26"/>
@@ -1747,48 +1747,48 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="J9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="K9" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="P9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="Q9" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="U9" s="48" t="s">
         <v>95</v>
-      </c>
-      <c r="R9" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="S9" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="T9" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="U9" s="48" t="s">
-        <v>96</v>
       </c>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>

</xml_diff>

<commit_message>
#update filed name in excel
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -759,89 +759,89 @@
     <xf numFmtId="37" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1169,167 +1169,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
     </row>
     <row r="2" spans="1:56">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="F3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="62" t="s">
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="52" t="s">
+      <c r="O3" s="51"/>
+      <c r="P3" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q3" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="56" t="s">
+      <c r="R3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="57"/>
-      <c r="T3" s="58" t="s">
+      <c r="S3" s="71"/>
+      <c r="T3" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="58" t="s">
+      <c r="U3" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="58" t="s">
+      <c r="V3" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="58" t="s">
+      <c r="W3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="58" t="s">
+      <c r="X3" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="63" t="s">
+      <c r="Y3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="54" t="s">
+      <c r="Z3" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="54" t="s">
+      <c r="AA3" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="50" t="s">
+      <c r="AB3" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="60" t="s">
+      <c r="AC3" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="60" t="s">
+      <c r="AD3" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AE3" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="50" t="s">
+      <c r="AF3" s="72" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:56">
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
       <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1348,31 +1348,31 @@
       <c r="O4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="59"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="53"/>
       <c r="R4" s="29" t="s">
         <v>63</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="55" t="s">
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="55" t="s">
+      <c r="AA4" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="51"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="51"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="77"/>
+      <c r="AD4" s="77"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
     </row>
     <row r="5" spans="1:56" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1472,10 +1472,10 @@
     <row r="6" spans="1:56" s="7" customFormat="1">
       <c r="A6" s="15"/>
       <c r="B6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>28</v>
@@ -1584,10 +1584,10 @@
     <row r="7" spans="1:56" s="7" customFormat="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>88</v>
@@ -1670,10 +1670,10 @@
     <row r="8" spans="1:56" s="7" customFormat="1">
       <c r="A8" s="15"/>
       <c r="B8" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>84</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>87</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>89</v>
@@ -1805,6 +1805,18 @@
   </sheetData>
   <autoFilter ref="B5:AF6"/>
   <mergeCells count="28">
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="Y3:Y4"/>
@@ -1821,18 +1833,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="U3:U4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#commit prod/hotfix/Update-Soa-Customer-Payment-History CR search pm datetime created->paymentdate
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Customer in payment history" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Customer in payment history'!$B$5:$AF$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Customer in payment history'!$B$5:$AG$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -330,6 +330,13 @@
   </si>
   <si>
     <t>{RangeDate}</t>
+  </si>
+  <si>
+    <t>{CombineNo}</t>
+  </si>
+  <si>
+    <t>Combine
+Billing</t>
   </si>
 </sst>
 </file>
@@ -642,7 +649,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,18 +766,48 @@
     <xf numFmtId="37" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="2" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="10" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -816,32 +853,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1129,207 +1142,212 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:BD9"/>
+  <dimension ref="A1:BE9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.7265625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="15.453125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="16" width="16.7265625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.26953125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="14.7265625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.81640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1796875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.81640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.453125" style="1" customWidth="1"/>
-    <col min="25" max="27" width="16.453125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.1796875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1796875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="12.1796875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="12.81640625" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.81640625" style="1"/>
+    <col min="14" max="16" width="16.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="1" customWidth="1"/>
+    <col min="18" max="19" width="14.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="16.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
+    <col min="31" max="32" width="12.140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.85546875" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56">
-      <c r="B1" s="56" t="s">
+    <row r="1" spans="1:57">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="50"/>
     </row>
-    <row r="2" spans="1:56">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="1:57">
+      <c r="B2" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="57"/>
-      <c r="AE2" s="57"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="79"/>
     </row>
-    <row r="3" spans="1:56" ht="15" customHeight="1">
-      <c r="B3" s="58" t="s">
+    <row r="3" spans="1:57" ht="15" customHeight="1">
+      <c r="B3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="50" t="s">
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="69" t="s">
+      <c r="O3" s="57"/>
+      <c r="P3" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="71"/>
-      <c r="T3" s="52" t="s">
+      <c r="S3" s="58"/>
+      <c r="T3" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="52" t="s">
+      <c r="V3" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="52" t="s">
+      <c r="X3" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="54" t="s">
+      <c r="Y3" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="74" t="s">
+      <c r="Z3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="74" t="s">
+      <c r="AA3" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="72" t="s">
+      <c r="AB3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="76" t="s">
+      <c r="AC3" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="76" t="s">
+      <c r="AD3" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="AE3" s="72" t="s">
+      <c r="AE3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="72" t="s">
+      <c r="AF3" s="51" t="s">
         <v>17</v>
       </c>
+      <c r="AG3" s="51" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:56">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
+    <row r="4" spans="1:57">
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
       <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1348,33 +1366,34 @@
       <c r="O4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="53"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="60"/>
       <c r="R4" s="29" t="s">
         <v>63</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="75" t="s">
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="75" t="s">
+      <c r="AA4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
     </row>
-    <row r="5" spans="1:56" s="6" customFormat="1">
+    <row r="5" spans="1:57" s="6" customFormat="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1468,8 +1487,11 @@
       <c r="AF5" s="5">
         <v>31</v>
       </c>
+      <c r="AG5" s="5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" s="7" customFormat="1">
+    <row r="6" spans="1:57" s="7" customFormat="1">
       <c r="A6" s="15"/>
       <c r="B6" s="30" t="s">
         <v>26</v>
@@ -1556,7 +1578,9 @@
       <c r="AF6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AG6" s="15"/>
+      <c r="AG6" s="22" t="s">
+        <v>99</v>
+      </c>
       <c r="AH6" s="15"/>
       <c r="AI6" s="15"/>
       <c r="AJ6" s="15"/>
@@ -1580,8 +1604,9 @@
       <c r="BB6" s="15"/>
       <c r="BC6" s="15"/>
       <c r="BD6" s="15"/>
+      <c r="BE6" s="15"/>
     </row>
-    <row r="7" spans="1:56" s="7" customFormat="1">
+    <row r="7" spans="1:57" s="7" customFormat="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>85</v>
@@ -1642,7 +1667,7 @@
       <c r="AD7" s="19"/>
       <c r="AE7" s="19"/>
       <c r="AF7" s="19"/>
-      <c r="AG7" s="15"/>
+      <c r="AG7" s="19"/>
       <c r="AH7" s="15"/>
       <c r="AI7" s="15"/>
       <c r="AJ7" s="15"/>
@@ -1666,8 +1691,9 @@
       <c r="BB7" s="15"/>
       <c r="BC7" s="15"/>
       <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
     </row>
-    <row r="8" spans="1:56" s="7" customFormat="1">
+    <row r="8" spans="1:57" s="7" customFormat="1">
       <c r="A8" s="15"/>
       <c r="B8" s="23" t="s">
         <v>87</v>
@@ -1718,7 +1744,7 @@
       </c>
       <c r="AE8" s="26"/>
       <c r="AF8" s="26"/>
-      <c r="AG8" s="15"/>
+      <c r="AG8" s="26"/>
       <c r="AH8" s="15"/>
       <c r="AI8" s="15"/>
       <c r="AJ8" s="15"/>
@@ -1742,8 +1768,9 @@
       <c r="BB8" s="15"/>
       <c r="BC8" s="15"/>
       <c r="BD8" s="15"/>
+      <c r="BE8" s="15"/>
     </row>
-    <row r="9" spans="1:56" s="14" customFormat="1">
+    <row r="9" spans="1:57" s="14" customFormat="1">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
@@ -1801,22 +1828,12 @@
       <c r="AD9" s="11"/>
       <c r="AE9" s="11"/>
       <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AF6"/>
-  <mergeCells count="28">
+  <autoFilter ref="B5:AG6"/>
+  <mergeCells count="29">
     <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="Y3:Y4"/>
@@ -1833,6 +1850,18 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="U3:U4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#update saleman hd obh and add saleman in adv amount rows
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210"/>
   </bookViews>
   <sheets>
     <sheet name="Customer in payment history" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -337,6 +337,9 @@
   <si>
     <t>Combine
 Billing</t>
+  </si>
+  <si>
+    <t>{SalesmanAdv}</t>
   </si>
 </sst>
 </file>
@@ -769,92 +772,92 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1151,203 +1154,203 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="15.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.7265625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15.453125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.26953125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="16" width="16.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="1" customWidth="1"/>
-    <col min="18" max="19" width="14.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" style="1" customWidth="1"/>
-    <col min="25" max="27" width="16.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="32" width="12.140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.85546875" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="1"/>
+    <col min="14" max="16" width="16.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.26953125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="14.7265625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1796875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="16.453125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.1796875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="1" customWidth="1"/>
+    <col min="31" max="32" width="12.1796875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.81640625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
       <c r="AF1" s="50"/>
     </row>
     <row r="2" spans="1:57">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67"/>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="79"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="51"/>
     </row>
     <row r="3" spans="1:57" ht="15" customHeight="1">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="63" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="55"/>
+      <c r="P3" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="57" t="s">
+      <c r="R3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="58"/>
-      <c r="T3" s="59" t="s">
+      <c r="S3" s="75"/>
+      <c r="T3" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="59" t="s">
+      <c r="U3" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="59" t="s">
+      <c r="V3" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="59" t="s">
+      <c r="W3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="59" t="s">
+      <c r="X3" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="64" t="s">
+      <c r="Y3" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="55" t="s">
+      <c r="Z3" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="55" t="s">
+      <c r="AA3" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="51" t="s">
+      <c r="AB3" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="61" t="s">
+      <c r="AC3" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="61" t="s">
+      <c r="AD3" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="AE3" s="51" t="s">
+      <c r="AE3" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="51" t="s">
+      <c r="AF3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AG3" s="51" t="s">
+      <c r="AG3" s="52" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:57">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1366,32 +1369,32 @@
       <c r="O4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="60"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="57"/>
       <c r="R4" s="29" t="s">
         <v>63</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="60"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="65"/>
-      <c r="Z4" s="56" t="s">
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="56" t="s">
+      <c r="AA4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="62"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52"/>
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="53"/>
+      <c r="AF4" s="53"/>
+      <c r="AG4" s="53"/>
     </row>
     <row r="5" spans="1:57" s="6" customFormat="1">
       <c r="B5" s="5">
@@ -1742,7 +1745,9 @@
       <c r="AD8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="AE8" s="26"/>
+      <c r="AE8" s="26" t="s">
+        <v>101</v>
+      </c>
       <c r="AF8" s="26"/>
       <c r="AG8" s="26"/>
       <c r="AH8" s="15"/>
@@ -1833,6 +1838,19 @@
   </sheetData>
   <autoFilter ref="B5:AG6"/>
   <mergeCells count="29">
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="T3:T4"/>
@@ -1849,19 +1867,6 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Prod/hotfix/18617 18519 update customer receivable obh
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Customer.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Customer in payment history" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Customer in payment history'!$B$5:$AH$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Customer in payment history'!$B$5:$AK$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>BÁO CÁO CÔNG NỢ KHÁCH HÀNG</t>
   </si>
@@ -347,6 +347,24 @@
   </si>
   <si>
     <t>{BillingNote}</t>
+  </si>
+  <si>
+    <t>Hạn thanh toán (OBH)</t>
+  </si>
+  <si>
+    <t>Ngày đến hạn (OBH)</t>
+  </si>
+  <si>
+    <t>Số ngày quá hạn (OBH)</t>
+  </si>
+  <si>
+    <t>{PaymentTermOBH}</t>
+  </si>
+  <si>
+    <t>{DueDateOBH}</t>
+  </si>
+  <si>
+    <t>{OverdueDaysOBH}</t>
   </si>
 </sst>
 </file>
@@ -785,17 +803,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1155,10 +1173,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:BF9"/>
+  <dimension ref="A1:BI9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
@@ -1185,16 +1203,19 @@
     <col min="22" max="22" width="10.140625" style="1" customWidth="1"/>
     <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
     <col min="24" max="24" width="9.42578125" style="1" customWidth="1"/>
-    <col min="25" max="27" width="16.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" customWidth="1"/>
-    <col min="31" max="33" width="12.140625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.85546875" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.85546875" style="1"/>
+    <col min="25" max="25" width="11.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" style="1" customWidth="1"/>
+    <col min="28" max="30" width="16.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="1" customWidth="1"/>
+    <col min="34" max="36" width="12.140625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="12.85546875" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:61">
       <c r="B1" s="59" t="s">
         <v>0</v>
       </c>
@@ -1227,10 +1248,13 @@
       <c r="AC1" s="59"/>
       <c r="AD1" s="59"/>
       <c r="AE1" s="59"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="52"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="52"/>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:61">
       <c r="B2" s="60" t="s">
         <v>98</v>
       </c>
@@ -1263,10 +1287,13 @@
       <c r="AC2" s="60"/>
       <c r="AD2" s="60"/>
       <c r="AE2" s="60"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
+      <c r="AF2" s="60"/>
+      <c r="AG2" s="60"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
     </row>
-    <row r="3" spans="1:58" ht="15" customHeight="1">
+    <row r="3" spans="1:61" ht="15" customHeight="1">
       <c r="B3" s="61" t="s">
         <v>1</v>
       </c>
@@ -1291,73 +1318,82 @@
       <c r="I3" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
       <c r="M3" s="74"/>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="54"/>
+      <c r="O3" s="56"/>
       <c r="P3" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="55" t="s">
+      <c r="Q3" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="54" t="s">
+      <c r="R3" s="56" t="s">
         <v>11</v>
       </c>
       <c r="S3" s="74"/>
-      <c r="T3" s="55" t="s">
+      <c r="T3" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="U3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="55" t="s">
+      <c r="V3" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="55" t="s">
+      <c r="W3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="55" t="s">
+      <c r="X3" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="57" t="s">
+      <c r="Y3" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z3" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA3" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB3" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="77" t="s">
+      <c r="AC3" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="77" t="s">
+      <c r="AD3" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="75" t="s">
+      <c r="AE3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="79" t="s">
+      <c r="AF3" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="79" t="s">
+      <c r="AG3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="AE3" s="75" t="s">
+      <c r="AH3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="75" t="s">
+      <c r="AI3" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="AG3" s="75" t="s">
+      <c r="AJ3" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="AH3" s="75" t="s">
+      <c r="AK3" s="75" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:61" ht="15" customHeight="1">
       <c r="B4" s="62"/>
       <c r="C4" s="63"/>
       <c r="D4" s="65"/>
@@ -1385,34 +1421,37 @@
         <v>23</v>
       </c>
       <c r="P4" s="73"/>
-      <c r="Q4" s="56"/>
+      <c r="Q4" s="54"/>
       <c r="R4" s="29" t="s">
         <v>63</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="78" t="s">
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="78" t="s">
+      <c r="AD4" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="80"/>
       <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="76"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
       <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
     </row>
-    <row r="5" spans="1:58" s="6" customFormat="1">
+    <row r="5" spans="1:61" s="6" customFormat="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1510,10 +1549,19 @@
         <v>32</v>
       </c>
       <c r="AH5" s="5">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>34</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>35</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:58" s="7" customFormat="1">
+    <row r="6" spans="1:61" s="7" customFormat="1">
       <c r="A6" s="15"/>
       <c r="B6" s="30" t="s">
         <v>26</v>
@@ -1576,39 +1624,45 @@
       <c r="X6" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="Y6" s="30" t="s">
+      <c r="Y6" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z6" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA6" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB6" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="Z6" s="30" t="s">
+      <c r="AC6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="AA6" s="30" t="s">
+      <c r="AD6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AB6" s="30" t="s">
+      <c r="AE6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AC6" s="22" t="s">
+      <c r="AF6" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="AD6" s="22" t="s">
+      <c r="AG6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AE6" s="22" t="s">
+      <c r="AH6" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AF6" s="22" t="s">
+      <c r="AI6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AG6" s="22" t="s">
+      <c r="AJ6" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="AH6" s="30" t="s">
+      <c r="AK6" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
       <c r="AN6" s="15"/>
@@ -1630,8 +1684,11 @@
       <c r="BD6" s="15"/>
       <c r="BE6" s="15"/>
       <c r="BF6" s="15"/>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="15"/>
+      <c r="BI6" s="15"/>
     </row>
-    <row r="7" spans="1:58" s="7" customFormat="1">
+    <row r="7" spans="1:61" s="7" customFormat="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>85</v>
@@ -1676,27 +1733,27 @@
       <c r="V7" s="42"/>
       <c r="W7" s="42"/>
       <c r="X7" s="42"/>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Z7" s="16" t="s">
+      <c r="AC7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AA7" s="16" t="s">
+      <c r="AD7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AB7" s="16" t="s">
+      <c r="AE7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
       <c r="AF7" s="19"/>
       <c r="AG7" s="19"/>
       <c r="AH7" s="19"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="15"/>
+      <c r="AI7" s="19"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
       <c r="AN7" s="15"/>
@@ -1718,8 +1775,11 @@
       <c r="BD7" s="15"/>
       <c r="BE7" s="15"/>
       <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="15"/>
+      <c r="BI7" s="15"/>
     </row>
-    <row r="8" spans="1:58" s="7" customFormat="1">
+    <row r="8" spans="1:61" s="7" customFormat="1">
       <c r="A8" s="15"/>
       <c r="B8" s="23" t="s">
         <v>87</v>
@@ -1760,23 +1820,23 @@
       <c r="V8" s="44"/>
       <c r="W8" s="44"/>
       <c r="X8" s="44"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
       <c r="AB8" s="26"/>
       <c r="AC8" s="26"/>
-      <c r="AD8" s="26" t="s">
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="AE8" s="26" t="s">
+      <c r="AH8" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="AF8" s="26"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="15"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15"/>
       <c r="AN8" s="15"/>
@@ -1798,8 +1858,11 @@
       <c r="BD8" s="15"/>
       <c r="BE8" s="15"/>
       <c r="BF8" s="15"/>
+      <c r="BG8" s="15"/>
+      <c r="BH8" s="15"/>
+      <c r="BI8" s="15"/>
     </row>
-    <row r="9" spans="1:58" s="14" customFormat="1">
+    <row r="9" spans="1:61" s="14" customFormat="1">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
@@ -1849,9 +1912,9 @@
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
       <c r="AB9" s="11"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
@@ -1859,29 +1922,30 @@
       <c r="AF9" s="11"/>
       <c r="AG9" s="11"/>
       <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AH6"/>
-  <mergeCells count="30">
+  <autoFilter ref="B5:AK6"/>
+  <mergeCells count="33">
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="B1:AE1"/>
-    <mergeCell ref="B2:AE2"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="B1:AH1"/>
+    <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -1893,6 +1957,11 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="U3:U4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="T3:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>